<commit_message>
1、sync code from svn
</commit_message>
<xml_diff>
--- a/Build/carcompare/WEB-INF/classes/static/static/templates/车型网车型数据搜集.xlsx
+++ b/Build/carcompare/WEB-INF/classes/static/static/templates/车型网车型数据搜集.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\01Work\01Project\08CarCompare\Code\CarCompare_UI\src\assets\templates\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="30" windowWidth="23715" windowHeight="8970"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>品牌</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -29,12 +34,16 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>配置型</t>
+    <t>车型数据</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>车型数据</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <t>配置型</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>品牌首字母</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -193,18 +202,49 @@
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -246,7 +286,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -281,7 +321,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -490,345 +530,346 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="12.75" style="4" customWidth="1"/>
     <col min="2" max="2" width="28.875" style="4" customWidth="1"/>
-    <col min="3" max="3" width="19.875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="39.625" style="4" customWidth="1"/>
-    <col min="5" max="256" width="9" style="4"/>
-    <col min="257" max="257" width="12.75" style="4" customWidth="1"/>
-    <col min="258" max="258" width="28.875" style="4" customWidth="1"/>
-    <col min="259" max="259" width="19.875" style="4" customWidth="1"/>
-    <col min="260" max="260" width="39.625" style="4" customWidth="1"/>
-    <col min="261" max="512" width="9" style="4"/>
-    <col min="513" max="513" width="12.75" style="4" customWidth="1"/>
-    <col min="514" max="514" width="28.875" style="4" customWidth="1"/>
-    <col min="515" max="515" width="19.875" style="4" customWidth="1"/>
-    <col min="516" max="516" width="39.625" style="4" customWidth="1"/>
-    <col min="517" max="768" width="9" style="4"/>
-    <col min="769" max="769" width="12.75" style="4" customWidth="1"/>
-    <col min="770" max="770" width="28.875" style="4" customWidth="1"/>
-    <col min="771" max="771" width="19.875" style="4" customWidth="1"/>
-    <col min="772" max="772" width="39.625" style="4" customWidth="1"/>
-    <col min="773" max="1024" width="9" style="4"/>
-    <col min="1025" max="1025" width="12.75" style="4" customWidth="1"/>
-    <col min="1026" max="1026" width="28.875" style="4" customWidth="1"/>
-    <col min="1027" max="1027" width="19.875" style="4" customWidth="1"/>
-    <col min="1028" max="1028" width="39.625" style="4" customWidth="1"/>
-    <col min="1029" max="1280" width="9" style="4"/>
-    <col min="1281" max="1281" width="12.75" style="4" customWidth="1"/>
-    <col min="1282" max="1282" width="28.875" style="4" customWidth="1"/>
-    <col min="1283" max="1283" width="19.875" style="4" customWidth="1"/>
-    <col min="1284" max="1284" width="39.625" style="4" customWidth="1"/>
-    <col min="1285" max="1536" width="9" style="4"/>
-    <col min="1537" max="1537" width="12.75" style="4" customWidth="1"/>
-    <col min="1538" max="1538" width="28.875" style="4" customWidth="1"/>
-    <col min="1539" max="1539" width="19.875" style="4" customWidth="1"/>
-    <col min="1540" max="1540" width="39.625" style="4" customWidth="1"/>
-    <col min="1541" max="1792" width="9" style="4"/>
-    <col min="1793" max="1793" width="12.75" style="4" customWidth="1"/>
-    <col min="1794" max="1794" width="28.875" style="4" customWidth="1"/>
-    <col min="1795" max="1795" width="19.875" style="4" customWidth="1"/>
-    <col min="1796" max="1796" width="39.625" style="4" customWidth="1"/>
-    <col min="1797" max="2048" width="9" style="4"/>
-    <col min="2049" max="2049" width="12.75" style="4" customWidth="1"/>
-    <col min="2050" max="2050" width="28.875" style="4" customWidth="1"/>
-    <col min="2051" max="2051" width="19.875" style="4" customWidth="1"/>
-    <col min="2052" max="2052" width="39.625" style="4" customWidth="1"/>
-    <col min="2053" max="2304" width="9" style="4"/>
-    <col min="2305" max="2305" width="12.75" style="4" customWidth="1"/>
-    <col min="2306" max="2306" width="28.875" style="4" customWidth="1"/>
-    <col min="2307" max="2307" width="19.875" style="4" customWidth="1"/>
-    <col min="2308" max="2308" width="39.625" style="4" customWidth="1"/>
-    <col min="2309" max="2560" width="9" style="4"/>
-    <col min="2561" max="2561" width="12.75" style="4" customWidth="1"/>
-    <col min="2562" max="2562" width="28.875" style="4" customWidth="1"/>
-    <col min="2563" max="2563" width="19.875" style="4" customWidth="1"/>
-    <col min="2564" max="2564" width="39.625" style="4" customWidth="1"/>
-    <col min="2565" max="2816" width="9" style="4"/>
-    <col min="2817" max="2817" width="12.75" style="4" customWidth="1"/>
-    <col min="2818" max="2818" width="28.875" style="4" customWidth="1"/>
-    <col min="2819" max="2819" width="19.875" style="4" customWidth="1"/>
-    <col min="2820" max="2820" width="39.625" style="4" customWidth="1"/>
-    <col min="2821" max="3072" width="9" style="4"/>
-    <col min="3073" max="3073" width="12.75" style="4" customWidth="1"/>
-    <col min="3074" max="3074" width="28.875" style="4" customWidth="1"/>
-    <col min="3075" max="3075" width="19.875" style="4" customWidth="1"/>
-    <col min="3076" max="3076" width="39.625" style="4" customWidth="1"/>
-    <col min="3077" max="3328" width="9" style="4"/>
-    <col min="3329" max="3329" width="12.75" style="4" customWidth="1"/>
-    <col min="3330" max="3330" width="28.875" style="4" customWidth="1"/>
-    <col min="3331" max="3331" width="19.875" style="4" customWidth="1"/>
-    <col min="3332" max="3332" width="39.625" style="4" customWidth="1"/>
-    <col min="3333" max="3584" width="9" style="4"/>
-    <col min="3585" max="3585" width="12.75" style="4" customWidth="1"/>
-    <col min="3586" max="3586" width="28.875" style="4" customWidth="1"/>
-    <col min="3587" max="3587" width="19.875" style="4" customWidth="1"/>
-    <col min="3588" max="3588" width="39.625" style="4" customWidth="1"/>
-    <col min="3589" max="3840" width="9" style="4"/>
-    <col min="3841" max="3841" width="12.75" style="4" customWidth="1"/>
-    <col min="3842" max="3842" width="28.875" style="4" customWidth="1"/>
-    <col min="3843" max="3843" width="19.875" style="4" customWidth="1"/>
-    <col min="3844" max="3844" width="39.625" style="4" customWidth="1"/>
-    <col min="3845" max="4096" width="9" style="4"/>
-    <col min="4097" max="4097" width="12.75" style="4" customWidth="1"/>
-    <col min="4098" max="4098" width="28.875" style="4" customWidth="1"/>
-    <col min="4099" max="4099" width="19.875" style="4" customWidth="1"/>
-    <col min="4100" max="4100" width="39.625" style="4" customWidth="1"/>
-    <col min="4101" max="4352" width="9" style="4"/>
-    <col min="4353" max="4353" width="12.75" style="4" customWidth="1"/>
-    <col min="4354" max="4354" width="28.875" style="4" customWidth="1"/>
-    <col min="4355" max="4355" width="19.875" style="4" customWidth="1"/>
-    <col min="4356" max="4356" width="39.625" style="4" customWidth="1"/>
-    <col min="4357" max="4608" width="9" style="4"/>
-    <col min="4609" max="4609" width="12.75" style="4" customWidth="1"/>
-    <col min="4610" max="4610" width="28.875" style="4" customWidth="1"/>
-    <col min="4611" max="4611" width="19.875" style="4" customWidth="1"/>
-    <col min="4612" max="4612" width="39.625" style="4" customWidth="1"/>
-    <col min="4613" max="4864" width="9" style="4"/>
-    <col min="4865" max="4865" width="12.75" style="4" customWidth="1"/>
-    <col min="4866" max="4866" width="28.875" style="4" customWidth="1"/>
-    <col min="4867" max="4867" width="19.875" style="4" customWidth="1"/>
-    <col min="4868" max="4868" width="39.625" style="4" customWidth="1"/>
-    <col min="4869" max="5120" width="9" style="4"/>
-    <col min="5121" max="5121" width="12.75" style="4" customWidth="1"/>
-    <col min="5122" max="5122" width="28.875" style="4" customWidth="1"/>
-    <col min="5123" max="5123" width="19.875" style="4" customWidth="1"/>
-    <col min="5124" max="5124" width="39.625" style="4" customWidth="1"/>
-    <col min="5125" max="5376" width="9" style="4"/>
-    <col min="5377" max="5377" width="12.75" style="4" customWidth="1"/>
-    <col min="5378" max="5378" width="28.875" style="4" customWidth="1"/>
-    <col min="5379" max="5379" width="19.875" style="4" customWidth="1"/>
-    <col min="5380" max="5380" width="39.625" style="4" customWidth="1"/>
-    <col min="5381" max="5632" width="9" style="4"/>
-    <col min="5633" max="5633" width="12.75" style="4" customWidth="1"/>
-    <col min="5634" max="5634" width="28.875" style="4" customWidth="1"/>
-    <col min="5635" max="5635" width="19.875" style="4" customWidth="1"/>
-    <col min="5636" max="5636" width="39.625" style="4" customWidth="1"/>
-    <col min="5637" max="5888" width="9" style="4"/>
-    <col min="5889" max="5889" width="12.75" style="4" customWidth="1"/>
-    <col min="5890" max="5890" width="28.875" style="4" customWidth="1"/>
-    <col min="5891" max="5891" width="19.875" style="4" customWidth="1"/>
-    <col min="5892" max="5892" width="39.625" style="4" customWidth="1"/>
-    <col min="5893" max="6144" width="9" style="4"/>
-    <col min="6145" max="6145" width="12.75" style="4" customWidth="1"/>
-    <col min="6146" max="6146" width="28.875" style="4" customWidth="1"/>
-    <col min="6147" max="6147" width="19.875" style="4" customWidth="1"/>
-    <col min="6148" max="6148" width="39.625" style="4" customWidth="1"/>
-    <col min="6149" max="6400" width="9" style="4"/>
-    <col min="6401" max="6401" width="12.75" style="4" customWidth="1"/>
-    <col min="6402" max="6402" width="28.875" style="4" customWidth="1"/>
-    <col min="6403" max="6403" width="19.875" style="4" customWidth="1"/>
-    <col min="6404" max="6404" width="39.625" style="4" customWidth="1"/>
-    <col min="6405" max="6656" width="9" style="4"/>
-    <col min="6657" max="6657" width="12.75" style="4" customWidth="1"/>
-    <col min="6658" max="6658" width="28.875" style="4" customWidth="1"/>
-    <col min="6659" max="6659" width="19.875" style="4" customWidth="1"/>
-    <col min="6660" max="6660" width="39.625" style="4" customWidth="1"/>
-    <col min="6661" max="6912" width="9" style="4"/>
-    <col min="6913" max="6913" width="12.75" style="4" customWidth="1"/>
-    <col min="6914" max="6914" width="28.875" style="4" customWidth="1"/>
-    <col min="6915" max="6915" width="19.875" style="4" customWidth="1"/>
-    <col min="6916" max="6916" width="39.625" style="4" customWidth="1"/>
-    <col min="6917" max="7168" width="9" style="4"/>
-    <col min="7169" max="7169" width="12.75" style="4" customWidth="1"/>
-    <col min="7170" max="7170" width="28.875" style="4" customWidth="1"/>
-    <col min="7171" max="7171" width="19.875" style="4" customWidth="1"/>
-    <col min="7172" max="7172" width="39.625" style="4" customWidth="1"/>
-    <col min="7173" max="7424" width="9" style="4"/>
-    <col min="7425" max="7425" width="12.75" style="4" customWidth="1"/>
-    <col min="7426" max="7426" width="28.875" style="4" customWidth="1"/>
-    <col min="7427" max="7427" width="19.875" style="4" customWidth="1"/>
-    <col min="7428" max="7428" width="39.625" style="4" customWidth="1"/>
-    <col min="7429" max="7680" width="9" style="4"/>
-    <col min="7681" max="7681" width="12.75" style="4" customWidth="1"/>
-    <col min="7682" max="7682" width="28.875" style="4" customWidth="1"/>
-    <col min="7683" max="7683" width="19.875" style="4" customWidth="1"/>
-    <col min="7684" max="7684" width="39.625" style="4" customWidth="1"/>
-    <col min="7685" max="7936" width="9" style="4"/>
-    <col min="7937" max="7937" width="12.75" style="4" customWidth="1"/>
-    <col min="7938" max="7938" width="28.875" style="4" customWidth="1"/>
-    <col min="7939" max="7939" width="19.875" style="4" customWidth="1"/>
-    <col min="7940" max="7940" width="39.625" style="4" customWidth="1"/>
-    <col min="7941" max="8192" width="9" style="4"/>
-    <col min="8193" max="8193" width="12.75" style="4" customWidth="1"/>
-    <col min="8194" max="8194" width="28.875" style="4" customWidth="1"/>
-    <col min="8195" max="8195" width="19.875" style="4" customWidth="1"/>
-    <col min="8196" max="8196" width="39.625" style="4" customWidth="1"/>
-    <col min="8197" max="8448" width="9" style="4"/>
-    <col min="8449" max="8449" width="12.75" style="4" customWidth="1"/>
-    <col min="8450" max="8450" width="28.875" style="4" customWidth="1"/>
-    <col min="8451" max="8451" width="19.875" style="4" customWidth="1"/>
-    <col min="8452" max="8452" width="39.625" style="4" customWidth="1"/>
-    <col min="8453" max="8704" width="9" style="4"/>
-    <col min="8705" max="8705" width="12.75" style="4" customWidth="1"/>
-    <col min="8706" max="8706" width="28.875" style="4" customWidth="1"/>
-    <col min="8707" max="8707" width="19.875" style="4" customWidth="1"/>
-    <col min="8708" max="8708" width="39.625" style="4" customWidth="1"/>
-    <col min="8709" max="8960" width="9" style="4"/>
-    <col min="8961" max="8961" width="12.75" style="4" customWidth="1"/>
-    <col min="8962" max="8962" width="28.875" style="4" customWidth="1"/>
-    <col min="8963" max="8963" width="19.875" style="4" customWidth="1"/>
-    <col min="8964" max="8964" width="39.625" style="4" customWidth="1"/>
-    <col min="8965" max="9216" width="9" style="4"/>
-    <col min="9217" max="9217" width="12.75" style="4" customWidth="1"/>
-    <col min="9218" max="9218" width="28.875" style="4" customWidth="1"/>
-    <col min="9219" max="9219" width="19.875" style="4" customWidth="1"/>
-    <col min="9220" max="9220" width="39.625" style="4" customWidth="1"/>
-    <col min="9221" max="9472" width="9" style="4"/>
-    <col min="9473" max="9473" width="12.75" style="4" customWidth="1"/>
-    <col min="9474" max="9474" width="28.875" style="4" customWidth="1"/>
-    <col min="9475" max="9475" width="19.875" style="4" customWidth="1"/>
-    <col min="9476" max="9476" width="39.625" style="4" customWidth="1"/>
-    <col min="9477" max="9728" width="9" style="4"/>
-    <col min="9729" max="9729" width="12.75" style="4" customWidth="1"/>
-    <col min="9730" max="9730" width="28.875" style="4" customWidth="1"/>
-    <col min="9731" max="9731" width="19.875" style="4" customWidth="1"/>
-    <col min="9732" max="9732" width="39.625" style="4" customWidth="1"/>
-    <col min="9733" max="9984" width="9" style="4"/>
-    <col min="9985" max="9985" width="12.75" style="4" customWidth="1"/>
-    <col min="9986" max="9986" width="28.875" style="4" customWidth="1"/>
-    <col min="9987" max="9987" width="19.875" style="4" customWidth="1"/>
-    <col min="9988" max="9988" width="39.625" style="4" customWidth="1"/>
-    <col min="9989" max="10240" width="9" style="4"/>
-    <col min="10241" max="10241" width="12.75" style="4" customWidth="1"/>
-    <col min="10242" max="10242" width="28.875" style="4" customWidth="1"/>
-    <col min="10243" max="10243" width="19.875" style="4" customWidth="1"/>
-    <col min="10244" max="10244" width="39.625" style="4" customWidth="1"/>
-    <col min="10245" max="10496" width="9" style="4"/>
-    <col min="10497" max="10497" width="12.75" style="4" customWidth="1"/>
-    <col min="10498" max="10498" width="28.875" style="4" customWidth="1"/>
-    <col min="10499" max="10499" width="19.875" style="4" customWidth="1"/>
-    <col min="10500" max="10500" width="39.625" style="4" customWidth="1"/>
-    <col min="10501" max="10752" width="9" style="4"/>
-    <col min="10753" max="10753" width="12.75" style="4" customWidth="1"/>
-    <col min="10754" max="10754" width="28.875" style="4" customWidth="1"/>
-    <col min="10755" max="10755" width="19.875" style="4" customWidth="1"/>
-    <col min="10756" max="10756" width="39.625" style="4" customWidth="1"/>
-    <col min="10757" max="11008" width="9" style="4"/>
-    <col min="11009" max="11009" width="12.75" style="4" customWidth="1"/>
-    <col min="11010" max="11010" width="28.875" style="4" customWidth="1"/>
-    <col min="11011" max="11011" width="19.875" style="4" customWidth="1"/>
-    <col min="11012" max="11012" width="39.625" style="4" customWidth="1"/>
-    <col min="11013" max="11264" width="9" style="4"/>
-    <col min="11265" max="11265" width="12.75" style="4" customWidth="1"/>
-    <col min="11266" max="11266" width="28.875" style="4" customWidth="1"/>
-    <col min="11267" max="11267" width="19.875" style="4" customWidth="1"/>
-    <col min="11268" max="11268" width="39.625" style="4" customWidth="1"/>
-    <col min="11269" max="11520" width="9" style="4"/>
-    <col min="11521" max="11521" width="12.75" style="4" customWidth="1"/>
-    <col min="11522" max="11522" width="28.875" style="4" customWidth="1"/>
-    <col min="11523" max="11523" width="19.875" style="4" customWidth="1"/>
-    <col min="11524" max="11524" width="39.625" style="4" customWidth="1"/>
-    <col min="11525" max="11776" width="9" style="4"/>
-    <col min="11777" max="11777" width="12.75" style="4" customWidth="1"/>
-    <col min="11778" max="11778" width="28.875" style="4" customWidth="1"/>
-    <col min="11779" max="11779" width="19.875" style="4" customWidth="1"/>
-    <col min="11780" max="11780" width="39.625" style="4" customWidth="1"/>
-    <col min="11781" max="12032" width="9" style="4"/>
-    <col min="12033" max="12033" width="12.75" style="4" customWidth="1"/>
-    <col min="12034" max="12034" width="28.875" style="4" customWidth="1"/>
-    <col min="12035" max="12035" width="19.875" style="4" customWidth="1"/>
-    <col min="12036" max="12036" width="39.625" style="4" customWidth="1"/>
-    <col min="12037" max="12288" width="9" style="4"/>
-    <col min="12289" max="12289" width="12.75" style="4" customWidth="1"/>
-    <col min="12290" max="12290" width="28.875" style="4" customWidth="1"/>
-    <col min="12291" max="12291" width="19.875" style="4" customWidth="1"/>
-    <col min="12292" max="12292" width="39.625" style="4" customWidth="1"/>
-    <col min="12293" max="12544" width="9" style="4"/>
-    <col min="12545" max="12545" width="12.75" style="4" customWidth="1"/>
-    <col min="12546" max="12546" width="28.875" style="4" customWidth="1"/>
-    <col min="12547" max="12547" width="19.875" style="4" customWidth="1"/>
-    <col min="12548" max="12548" width="39.625" style="4" customWidth="1"/>
-    <col min="12549" max="12800" width="9" style="4"/>
-    <col min="12801" max="12801" width="12.75" style="4" customWidth="1"/>
-    <col min="12802" max="12802" width="28.875" style="4" customWidth="1"/>
-    <col min="12803" max="12803" width="19.875" style="4" customWidth="1"/>
-    <col min="12804" max="12804" width="39.625" style="4" customWidth="1"/>
-    <col min="12805" max="13056" width="9" style="4"/>
-    <col min="13057" max="13057" width="12.75" style="4" customWidth="1"/>
-    <col min="13058" max="13058" width="28.875" style="4" customWidth="1"/>
-    <col min="13059" max="13059" width="19.875" style="4" customWidth="1"/>
-    <col min="13060" max="13060" width="39.625" style="4" customWidth="1"/>
-    <col min="13061" max="13312" width="9" style="4"/>
-    <col min="13313" max="13313" width="12.75" style="4" customWidth="1"/>
-    <col min="13314" max="13314" width="28.875" style="4" customWidth="1"/>
-    <col min="13315" max="13315" width="19.875" style="4" customWidth="1"/>
-    <col min="13316" max="13316" width="39.625" style="4" customWidth="1"/>
-    <col min="13317" max="13568" width="9" style="4"/>
-    <col min="13569" max="13569" width="12.75" style="4" customWidth="1"/>
-    <col min="13570" max="13570" width="28.875" style="4" customWidth="1"/>
-    <col min="13571" max="13571" width="19.875" style="4" customWidth="1"/>
-    <col min="13572" max="13572" width="39.625" style="4" customWidth="1"/>
-    <col min="13573" max="13824" width="9" style="4"/>
-    <col min="13825" max="13825" width="12.75" style="4" customWidth="1"/>
-    <col min="13826" max="13826" width="28.875" style="4" customWidth="1"/>
-    <col min="13827" max="13827" width="19.875" style="4" customWidth="1"/>
-    <col min="13828" max="13828" width="39.625" style="4" customWidth="1"/>
-    <col min="13829" max="14080" width="9" style="4"/>
-    <col min="14081" max="14081" width="12.75" style="4" customWidth="1"/>
-    <col min="14082" max="14082" width="28.875" style="4" customWidth="1"/>
-    <col min="14083" max="14083" width="19.875" style="4" customWidth="1"/>
-    <col min="14084" max="14084" width="39.625" style="4" customWidth="1"/>
-    <col min="14085" max="14336" width="9" style="4"/>
-    <col min="14337" max="14337" width="12.75" style="4" customWidth="1"/>
-    <col min="14338" max="14338" width="28.875" style="4" customWidth="1"/>
-    <col min="14339" max="14339" width="19.875" style="4" customWidth="1"/>
-    <col min="14340" max="14340" width="39.625" style="4" customWidth="1"/>
-    <col min="14341" max="14592" width="9" style="4"/>
-    <col min="14593" max="14593" width="12.75" style="4" customWidth="1"/>
-    <col min="14594" max="14594" width="28.875" style="4" customWidth="1"/>
-    <col min="14595" max="14595" width="19.875" style="4" customWidth="1"/>
-    <col min="14596" max="14596" width="39.625" style="4" customWidth="1"/>
-    <col min="14597" max="14848" width="9" style="4"/>
-    <col min="14849" max="14849" width="12.75" style="4" customWidth="1"/>
-    <col min="14850" max="14850" width="28.875" style="4" customWidth="1"/>
-    <col min="14851" max="14851" width="19.875" style="4" customWidth="1"/>
-    <col min="14852" max="14852" width="39.625" style="4" customWidth="1"/>
-    <col min="14853" max="15104" width="9" style="4"/>
-    <col min="15105" max="15105" width="12.75" style="4" customWidth="1"/>
-    <col min="15106" max="15106" width="28.875" style="4" customWidth="1"/>
-    <col min="15107" max="15107" width="19.875" style="4" customWidth="1"/>
-    <col min="15108" max="15108" width="39.625" style="4" customWidth="1"/>
-    <col min="15109" max="15360" width="9" style="4"/>
-    <col min="15361" max="15361" width="12.75" style="4" customWidth="1"/>
-    <col min="15362" max="15362" width="28.875" style="4" customWidth="1"/>
-    <col min="15363" max="15363" width="19.875" style="4" customWidth="1"/>
-    <col min="15364" max="15364" width="39.625" style="4" customWidth="1"/>
-    <col min="15365" max="15616" width="9" style="4"/>
-    <col min="15617" max="15617" width="12.75" style="4" customWidth="1"/>
-    <col min="15618" max="15618" width="28.875" style="4" customWidth="1"/>
-    <col min="15619" max="15619" width="19.875" style="4" customWidth="1"/>
-    <col min="15620" max="15620" width="39.625" style="4" customWidth="1"/>
-    <col min="15621" max="15872" width="9" style="4"/>
-    <col min="15873" max="15873" width="12.75" style="4" customWidth="1"/>
-    <col min="15874" max="15874" width="28.875" style="4" customWidth="1"/>
-    <col min="15875" max="15875" width="19.875" style="4" customWidth="1"/>
-    <col min="15876" max="15876" width="39.625" style="4" customWidth="1"/>
-    <col min="15877" max="16128" width="9" style="4"/>
-    <col min="16129" max="16129" width="12.75" style="4" customWidth="1"/>
-    <col min="16130" max="16130" width="28.875" style="4" customWidth="1"/>
-    <col min="16131" max="16131" width="19.875" style="4" customWidth="1"/>
-    <col min="16132" max="16132" width="39.625" style="4" customWidth="1"/>
-    <col min="16133" max="16384" width="9" style="4"/>
+    <col min="3" max="4" width="19.875" style="4" customWidth="1"/>
+    <col min="5" max="5" width="39.625" style="4" customWidth="1"/>
+    <col min="6" max="257" width="9" style="4"/>
+    <col min="258" max="258" width="12.75" style="4" customWidth="1"/>
+    <col min="259" max="259" width="28.875" style="4" customWidth="1"/>
+    <col min="260" max="260" width="19.875" style="4" customWidth="1"/>
+    <col min="261" max="261" width="39.625" style="4" customWidth="1"/>
+    <col min="262" max="513" width="9" style="4"/>
+    <col min="514" max="514" width="12.75" style="4" customWidth="1"/>
+    <col min="515" max="515" width="28.875" style="4" customWidth="1"/>
+    <col min="516" max="516" width="19.875" style="4" customWidth="1"/>
+    <col min="517" max="517" width="39.625" style="4" customWidth="1"/>
+    <col min="518" max="769" width="9" style="4"/>
+    <col min="770" max="770" width="12.75" style="4" customWidth="1"/>
+    <col min="771" max="771" width="28.875" style="4" customWidth="1"/>
+    <col min="772" max="772" width="19.875" style="4" customWidth="1"/>
+    <col min="773" max="773" width="39.625" style="4" customWidth="1"/>
+    <col min="774" max="1025" width="9" style="4"/>
+    <col min="1026" max="1026" width="12.75" style="4" customWidth="1"/>
+    <col min="1027" max="1027" width="28.875" style="4" customWidth="1"/>
+    <col min="1028" max="1028" width="19.875" style="4" customWidth="1"/>
+    <col min="1029" max="1029" width="39.625" style="4" customWidth="1"/>
+    <col min="1030" max="1281" width="9" style="4"/>
+    <col min="1282" max="1282" width="12.75" style="4" customWidth="1"/>
+    <col min="1283" max="1283" width="28.875" style="4" customWidth="1"/>
+    <col min="1284" max="1284" width="19.875" style="4" customWidth="1"/>
+    <col min="1285" max="1285" width="39.625" style="4" customWidth="1"/>
+    <col min="1286" max="1537" width="9" style="4"/>
+    <col min="1538" max="1538" width="12.75" style="4" customWidth="1"/>
+    <col min="1539" max="1539" width="28.875" style="4" customWidth="1"/>
+    <col min="1540" max="1540" width="19.875" style="4" customWidth="1"/>
+    <col min="1541" max="1541" width="39.625" style="4" customWidth="1"/>
+    <col min="1542" max="1793" width="9" style="4"/>
+    <col min="1794" max="1794" width="12.75" style="4" customWidth="1"/>
+    <col min="1795" max="1795" width="28.875" style="4" customWidth="1"/>
+    <col min="1796" max="1796" width="19.875" style="4" customWidth="1"/>
+    <col min="1797" max="1797" width="39.625" style="4" customWidth="1"/>
+    <col min="1798" max="2049" width="9" style="4"/>
+    <col min="2050" max="2050" width="12.75" style="4" customWidth="1"/>
+    <col min="2051" max="2051" width="28.875" style="4" customWidth="1"/>
+    <col min="2052" max="2052" width="19.875" style="4" customWidth="1"/>
+    <col min="2053" max="2053" width="39.625" style="4" customWidth="1"/>
+    <col min="2054" max="2305" width="9" style="4"/>
+    <col min="2306" max="2306" width="12.75" style="4" customWidth="1"/>
+    <col min="2307" max="2307" width="28.875" style="4" customWidth="1"/>
+    <col min="2308" max="2308" width="19.875" style="4" customWidth="1"/>
+    <col min="2309" max="2309" width="39.625" style="4" customWidth="1"/>
+    <col min="2310" max="2561" width="9" style="4"/>
+    <col min="2562" max="2562" width="12.75" style="4" customWidth="1"/>
+    <col min="2563" max="2563" width="28.875" style="4" customWidth="1"/>
+    <col min="2564" max="2564" width="19.875" style="4" customWidth="1"/>
+    <col min="2565" max="2565" width="39.625" style="4" customWidth="1"/>
+    <col min="2566" max="2817" width="9" style="4"/>
+    <col min="2818" max="2818" width="12.75" style="4" customWidth="1"/>
+    <col min="2819" max="2819" width="28.875" style="4" customWidth="1"/>
+    <col min="2820" max="2820" width="19.875" style="4" customWidth="1"/>
+    <col min="2821" max="2821" width="39.625" style="4" customWidth="1"/>
+    <col min="2822" max="3073" width="9" style="4"/>
+    <col min="3074" max="3074" width="12.75" style="4" customWidth="1"/>
+    <col min="3075" max="3075" width="28.875" style="4" customWidth="1"/>
+    <col min="3076" max="3076" width="19.875" style="4" customWidth="1"/>
+    <col min="3077" max="3077" width="39.625" style="4" customWidth="1"/>
+    <col min="3078" max="3329" width="9" style="4"/>
+    <col min="3330" max="3330" width="12.75" style="4" customWidth="1"/>
+    <col min="3331" max="3331" width="28.875" style="4" customWidth="1"/>
+    <col min="3332" max="3332" width="19.875" style="4" customWidth="1"/>
+    <col min="3333" max="3333" width="39.625" style="4" customWidth="1"/>
+    <col min="3334" max="3585" width="9" style="4"/>
+    <col min="3586" max="3586" width="12.75" style="4" customWidth="1"/>
+    <col min="3587" max="3587" width="28.875" style="4" customWidth="1"/>
+    <col min="3588" max="3588" width="19.875" style="4" customWidth="1"/>
+    <col min="3589" max="3589" width="39.625" style="4" customWidth="1"/>
+    <col min="3590" max="3841" width="9" style="4"/>
+    <col min="3842" max="3842" width="12.75" style="4" customWidth="1"/>
+    <col min="3843" max="3843" width="28.875" style="4" customWidth="1"/>
+    <col min="3844" max="3844" width="19.875" style="4" customWidth="1"/>
+    <col min="3845" max="3845" width="39.625" style="4" customWidth="1"/>
+    <col min="3846" max="4097" width="9" style="4"/>
+    <col min="4098" max="4098" width="12.75" style="4" customWidth="1"/>
+    <col min="4099" max="4099" width="28.875" style="4" customWidth="1"/>
+    <col min="4100" max="4100" width="19.875" style="4" customWidth="1"/>
+    <col min="4101" max="4101" width="39.625" style="4" customWidth="1"/>
+    <col min="4102" max="4353" width="9" style="4"/>
+    <col min="4354" max="4354" width="12.75" style="4" customWidth="1"/>
+    <col min="4355" max="4355" width="28.875" style="4" customWidth="1"/>
+    <col min="4356" max="4356" width="19.875" style="4" customWidth="1"/>
+    <col min="4357" max="4357" width="39.625" style="4" customWidth="1"/>
+    <col min="4358" max="4609" width="9" style="4"/>
+    <col min="4610" max="4610" width="12.75" style="4" customWidth="1"/>
+    <col min="4611" max="4611" width="28.875" style="4" customWidth="1"/>
+    <col min="4612" max="4612" width="19.875" style="4" customWidth="1"/>
+    <col min="4613" max="4613" width="39.625" style="4" customWidth="1"/>
+    <col min="4614" max="4865" width="9" style="4"/>
+    <col min="4866" max="4866" width="12.75" style="4" customWidth="1"/>
+    <col min="4867" max="4867" width="28.875" style="4" customWidth="1"/>
+    <col min="4868" max="4868" width="19.875" style="4" customWidth="1"/>
+    <col min="4869" max="4869" width="39.625" style="4" customWidth="1"/>
+    <col min="4870" max="5121" width="9" style="4"/>
+    <col min="5122" max="5122" width="12.75" style="4" customWidth="1"/>
+    <col min="5123" max="5123" width="28.875" style="4" customWidth="1"/>
+    <col min="5124" max="5124" width="19.875" style="4" customWidth="1"/>
+    <col min="5125" max="5125" width="39.625" style="4" customWidth="1"/>
+    <col min="5126" max="5377" width="9" style="4"/>
+    <col min="5378" max="5378" width="12.75" style="4" customWidth="1"/>
+    <col min="5379" max="5379" width="28.875" style="4" customWidth="1"/>
+    <col min="5380" max="5380" width="19.875" style="4" customWidth="1"/>
+    <col min="5381" max="5381" width="39.625" style="4" customWidth="1"/>
+    <col min="5382" max="5633" width="9" style="4"/>
+    <col min="5634" max="5634" width="12.75" style="4" customWidth="1"/>
+    <col min="5635" max="5635" width="28.875" style="4" customWidth="1"/>
+    <col min="5636" max="5636" width="19.875" style="4" customWidth="1"/>
+    <col min="5637" max="5637" width="39.625" style="4" customWidth="1"/>
+    <col min="5638" max="5889" width="9" style="4"/>
+    <col min="5890" max="5890" width="12.75" style="4" customWidth="1"/>
+    <col min="5891" max="5891" width="28.875" style="4" customWidth="1"/>
+    <col min="5892" max="5892" width="19.875" style="4" customWidth="1"/>
+    <col min="5893" max="5893" width="39.625" style="4" customWidth="1"/>
+    <col min="5894" max="6145" width="9" style="4"/>
+    <col min="6146" max="6146" width="12.75" style="4" customWidth="1"/>
+    <col min="6147" max="6147" width="28.875" style="4" customWidth="1"/>
+    <col min="6148" max="6148" width="19.875" style="4" customWidth="1"/>
+    <col min="6149" max="6149" width="39.625" style="4" customWidth="1"/>
+    <col min="6150" max="6401" width="9" style="4"/>
+    <col min="6402" max="6402" width="12.75" style="4" customWidth="1"/>
+    <col min="6403" max="6403" width="28.875" style="4" customWidth="1"/>
+    <col min="6404" max="6404" width="19.875" style="4" customWidth="1"/>
+    <col min="6405" max="6405" width="39.625" style="4" customWidth="1"/>
+    <col min="6406" max="6657" width="9" style="4"/>
+    <col min="6658" max="6658" width="12.75" style="4" customWidth="1"/>
+    <col min="6659" max="6659" width="28.875" style="4" customWidth="1"/>
+    <col min="6660" max="6660" width="19.875" style="4" customWidth="1"/>
+    <col min="6661" max="6661" width="39.625" style="4" customWidth="1"/>
+    <col min="6662" max="6913" width="9" style="4"/>
+    <col min="6914" max="6914" width="12.75" style="4" customWidth="1"/>
+    <col min="6915" max="6915" width="28.875" style="4" customWidth="1"/>
+    <col min="6916" max="6916" width="19.875" style="4" customWidth="1"/>
+    <col min="6917" max="6917" width="39.625" style="4" customWidth="1"/>
+    <col min="6918" max="7169" width="9" style="4"/>
+    <col min="7170" max="7170" width="12.75" style="4" customWidth="1"/>
+    <col min="7171" max="7171" width="28.875" style="4" customWidth="1"/>
+    <col min="7172" max="7172" width="19.875" style="4" customWidth="1"/>
+    <col min="7173" max="7173" width="39.625" style="4" customWidth="1"/>
+    <col min="7174" max="7425" width="9" style="4"/>
+    <col min="7426" max="7426" width="12.75" style="4" customWidth="1"/>
+    <col min="7427" max="7427" width="28.875" style="4" customWidth="1"/>
+    <col min="7428" max="7428" width="19.875" style="4" customWidth="1"/>
+    <col min="7429" max="7429" width="39.625" style="4" customWidth="1"/>
+    <col min="7430" max="7681" width="9" style="4"/>
+    <col min="7682" max="7682" width="12.75" style="4" customWidth="1"/>
+    <col min="7683" max="7683" width="28.875" style="4" customWidth="1"/>
+    <col min="7684" max="7684" width="19.875" style="4" customWidth="1"/>
+    <col min="7685" max="7685" width="39.625" style="4" customWidth="1"/>
+    <col min="7686" max="7937" width="9" style="4"/>
+    <col min="7938" max="7938" width="12.75" style="4" customWidth="1"/>
+    <col min="7939" max="7939" width="28.875" style="4" customWidth="1"/>
+    <col min="7940" max="7940" width="19.875" style="4" customWidth="1"/>
+    <col min="7941" max="7941" width="39.625" style="4" customWidth="1"/>
+    <col min="7942" max="8193" width="9" style="4"/>
+    <col min="8194" max="8194" width="12.75" style="4" customWidth="1"/>
+    <col min="8195" max="8195" width="28.875" style="4" customWidth="1"/>
+    <col min="8196" max="8196" width="19.875" style="4" customWidth="1"/>
+    <col min="8197" max="8197" width="39.625" style="4" customWidth="1"/>
+    <col min="8198" max="8449" width="9" style="4"/>
+    <col min="8450" max="8450" width="12.75" style="4" customWidth="1"/>
+    <col min="8451" max="8451" width="28.875" style="4" customWidth="1"/>
+    <col min="8452" max="8452" width="19.875" style="4" customWidth="1"/>
+    <col min="8453" max="8453" width="39.625" style="4" customWidth="1"/>
+    <col min="8454" max="8705" width="9" style="4"/>
+    <col min="8706" max="8706" width="12.75" style="4" customWidth="1"/>
+    <col min="8707" max="8707" width="28.875" style="4" customWidth="1"/>
+    <col min="8708" max="8708" width="19.875" style="4" customWidth="1"/>
+    <col min="8709" max="8709" width="39.625" style="4" customWidth="1"/>
+    <col min="8710" max="8961" width="9" style="4"/>
+    <col min="8962" max="8962" width="12.75" style="4" customWidth="1"/>
+    <col min="8963" max="8963" width="28.875" style="4" customWidth="1"/>
+    <col min="8964" max="8964" width="19.875" style="4" customWidth="1"/>
+    <col min="8965" max="8965" width="39.625" style="4" customWidth="1"/>
+    <col min="8966" max="9217" width="9" style="4"/>
+    <col min="9218" max="9218" width="12.75" style="4" customWidth="1"/>
+    <col min="9219" max="9219" width="28.875" style="4" customWidth="1"/>
+    <col min="9220" max="9220" width="19.875" style="4" customWidth="1"/>
+    <col min="9221" max="9221" width="39.625" style="4" customWidth="1"/>
+    <col min="9222" max="9473" width="9" style="4"/>
+    <col min="9474" max="9474" width="12.75" style="4" customWidth="1"/>
+    <col min="9475" max="9475" width="28.875" style="4" customWidth="1"/>
+    <col min="9476" max="9476" width="19.875" style="4" customWidth="1"/>
+    <col min="9477" max="9477" width="39.625" style="4" customWidth="1"/>
+    <col min="9478" max="9729" width="9" style="4"/>
+    <col min="9730" max="9730" width="12.75" style="4" customWidth="1"/>
+    <col min="9731" max="9731" width="28.875" style="4" customWidth="1"/>
+    <col min="9732" max="9732" width="19.875" style="4" customWidth="1"/>
+    <col min="9733" max="9733" width="39.625" style="4" customWidth="1"/>
+    <col min="9734" max="9985" width="9" style="4"/>
+    <col min="9986" max="9986" width="12.75" style="4" customWidth="1"/>
+    <col min="9987" max="9987" width="28.875" style="4" customWidth="1"/>
+    <col min="9988" max="9988" width="19.875" style="4" customWidth="1"/>
+    <col min="9989" max="9989" width="39.625" style="4" customWidth="1"/>
+    <col min="9990" max="10241" width="9" style="4"/>
+    <col min="10242" max="10242" width="12.75" style="4" customWidth="1"/>
+    <col min="10243" max="10243" width="28.875" style="4" customWidth="1"/>
+    <col min="10244" max="10244" width="19.875" style="4" customWidth="1"/>
+    <col min="10245" max="10245" width="39.625" style="4" customWidth="1"/>
+    <col min="10246" max="10497" width="9" style="4"/>
+    <col min="10498" max="10498" width="12.75" style="4" customWidth="1"/>
+    <col min="10499" max="10499" width="28.875" style="4" customWidth="1"/>
+    <col min="10500" max="10500" width="19.875" style="4" customWidth="1"/>
+    <col min="10501" max="10501" width="39.625" style="4" customWidth="1"/>
+    <col min="10502" max="10753" width="9" style="4"/>
+    <col min="10754" max="10754" width="12.75" style="4" customWidth="1"/>
+    <col min="10755" max="10755" width="28.875" style="4" customWidth="1"/>
+    <col min="10756" max="10756" width="19.875" style="4" customWidth="1"/>
+    <col min="10757" max="10757" width="39.625" style="4" customWidth="1"/>
+    <col min="10758" max="11009" width="9" style="4"/>
+    <col min="11010" max="11010" width="12.75" style="4" customWidth="1"/>
+    <col min="11011" max="11011" width="28.875" style="4" customWidth="1"/>
+    <col min="11012" max="11012" width="19.875" style="4" customWidth="1"/>
+    <col min="11013" max="11013" width="39.625" style="4" customWidth="1"/>
+    <col min="11014" max="11265" width="9" style="4"/>
+    <col min="11266" max="11266" width="12.75" style="4" customWidth="1"/>
+    <col min="11267" max="11267" width="28.875" style="4" customWidth="1"/>
+    <col min="11268" max="11268" width="19.875" style="4" customWidth="1"/>
+    <col min="11269" max="11269" width="39.625" style="4" customWidth="1"/>
+    <col min="11270" max="11521" width="9" style="4"/>
+    <col min="11522" max="11522" width="12.75" style="4" customWidth="1"/>
+    <col min="11523" max="11523" width="28.875" style="4" customWidth="1"/>
+    <col min="11524" max="11524" width="19.875" style="4" customWidth="1"/>
+    <col min="11525" max="11525" width="39.625" style="4" customWidth="1"/>
+    <col min="11526" max="11777" width="9" style="4"/>
+    <col min="11778" max="11778" width="12.75" style="4" customWidth="1"/>
+    <col min="11779" max="11779" width="28.875" style="4" customWidth="1"/>
+    <col min="11780" max="11780" width="19.875" style="4" customWidth="1"/>
+    <col min="11781" max="11781" width="39.625" style="4" customWidth="1"/>
+    <col min="11782" max="12033" width="9" style="4"/>
+    <col min="12034" max="12034" width="12.75" style="4" customWidth="1"/>
+    <col min="12035" max="12035" width="28.875" style="4" customWidth="1"/>
+    <col min="12036" max="12036" width="19.875" style="4" customWidth="1"/>
+    <col min="12037" max="12037" width="39.625" style="4" customWidth="1"/>
+    <col min="12038" max="12289" width="9" style="4"/>
+    <col min="12290" max="12290" width="12.75" style="4" customWidth="1"/>
+    <col min="12291" max="12291" width="28.875" style="4" customWidth="1"/>
+    <col min="12292" max="12292" width="19.875" style="4" customWidth="1"/>
+    <col min="12293" max="12293" width="39.625" style="4" customWidth="1"/>
+    <col min="12294" max="12545" width="9" style="4"/>
+    <col min="12546" max="12546" width="12.75" style="4" customWidth="1"/>
+    <col min="12547" max="12547" width="28.875" style="4" customWidth="1"/>
+    <col min="12548" max="12548" width="19.875" style="4" customWidth="1"/>
+    <col min="12549" max="12549" width="39.625" style="4" customWidth="1"/>
+    <col min="12550" max="12801" width="9" style="4"/>
+    <col min="12802" max="12802" width="12.75" style="4" customWidth="1"/>
+    <col min="12803" max="12803" width="28.875" style="4" customWidth="1"/>
+    <col min="12804" max="12804" width="19.875" style="4" customWidth="1"/>
+    <col min="12805" max="12805" width="39.625" style="4" customWidth="1"/>
+    <col min="12806" max="13057" width="9" style="4"/>
+    <col min="13058" max="13058" width="12.75" style="4" customWidth="1"/>
+    <col min="13059" max="13059" width="28.875" style="4" customWidth="1"/>
+    <col min="13060" max="13060" width="19.875" style="4" customWidth="1"/>
+    <col min="13061" max="13061" width="39.625" style="4" customWidth="1"/>
+    <col min="13062" max="13313" width="9" style="4"/>
+    <col min="13314" max="13314" width="12.75" style="4" customWidth="1"/>
+    <col min="13315" max="13315" width="28.875" style="4" customWidth="1"/>
+    <col min="13316" max="13316" width="19.875" style="4" customWidth="1"/>
+    <col min="13317" max="13317" width="39.625" style="4" customWidth="1"/>
+    <col min="13318" max="13569" width="9" style="4"/>
+    <col min="13570" max="13570" width="12.75" style="4" customWidth="1"/>
+    <col min="13571" max="13571" width="28.875" style="4" customWidth="1"/>
+    <col min="13572" max="13572" width="19.875" style="4" customWidth="1"/>
+    <col min="13573" max="13573" width="39.625" style="4" customWidth="1"/>
+    <col min="13574" max="13825" width="9" style="4"/>
+    <col min="13826" max="13826" width="12.75" style="4" customWidth="1"/>
+    <col min="13827" max="13827" width="28.875" style="4" customWidth="1"/>
+    <col min="13828" max="13828" width="19.875" style="4" customWidth="1"/>
+    <col min="13829" max="13829" width="39.625" style="4" customWidth="1"/>
+    <col min="13830" max="14081" width="9" style="4"/>
+    <col min="14082" max="14082" width="12.75" style="4" customWidth="1"/>
+    <col min="14083" max="14083" width="28.875" style="4" customWidth="1"/>
+    <col min="14084" max="14084" width="19.875" style="4" customWidth="1"/>
+    <col min="14085" max="14085" width="39.625" style="4" customWidth="1"/>
+    <col min="14086" max="14337" width="9" style="4"/>
+    <col min="14338" max="14338" width="12.75" style="4" customWidth="1"/>
+    <col min="14339" max="14339" width="28.875" style="4" customWidth="1"/>
+    <col min="14340" max="14340" width="19.875" style="4" customWidth="1"/>
+    <col min="14341" max="14341" width="39.625" style="4" customWidth="1"/>
+    <col min="14342" max="14593" width="9" style="4"/>
+    <col min="14594" max="14594" width="12.75" style="4" customWidth="1"/>
+    <col min="14595" max="14595" width="28.875" style="4" customWidth="1"/>
+    <col min="14596" max="14596" width="19.875" style="4" customWidth="1"/>
+    <col min="14597" max="14597" width="39.625" style="4" customWidth="1"/>
+    <col min="14598" max="14849" width="9" style="4"/>
+    <col min="14850" max="14850" width="12.75" style="4" customWidth="1"/>
+    <col min="14851" max="14851" width="28.875" style="4" customWidth="1"/>
+    <col min="14852" max="14852" width="19.875" style="4" customWidth="1"/>
+    <col min="14853" max="14853" width="39.625" style="4" customWidth="1"/>
+    <col min="14854" max="15105" width="9" style="4"/>
+    <col min="15106" max="15106" width="12.75" style="4" customWidth="1"/>
+    <col min="15107" max="15107" width="28.875" style="4" customWidth="1"/>
+    <col min="15108" max="15108" width="19.875" style="4" customWidth="1"/>
+    <col min="15109" max="15109" width="39.625" style="4" customWidth="1"/>
+    <col min="15110" max="15361" width="9" style="4"/>
+    <col min="15362" max="15362" width="12.75" style="4" customWidth="1"/>
+    <col min="15363" max="15363" width="28.875" style="4" customWidth="1"/>
+    <col min="15364" max="15364" width="19.875" style="4" customWidth="1"/>
+    <col min="15365" max="15365" width="39.625" style="4" customWidth="1"/>
+    <col min="15366" max="15617" width="9" style="4"/>
+    <col min="15618" max="15618" width="12.75" style="4" customWidth="1"/>
+    <col min="15619" max="15619" width="28.875" style="4" customWidth="1"/>
+    <col min="15620" max="15620" width="19.875" style="4" customWidth="1"/>
+    <col min="15621" max="15621" width="39.625" style="4" customWidth="1"/>
+    <col min="15622" max="15873" width="9" style="4"/>
+    <col min="15874" max="15874" width="12.75" style="4" customWidth="1"/>
+    <col min="15875" max="15875" width="28.875" style="4" customWidth="1"/>
+    <col min="15876" max="15876" width="19.875" style="4" customWidth="1"/>
+    <col min="15877" max="15877" width="39.625" style="4" customWidth="1"/>
+    <col min="15878" max="16129" width="9" style="4"/>
+    <col min="16130" max="16130" width="12.75" style="4" customWidth="1"/>
+    <col min="16131" max="16131" width="28.875" style="4" customWidth="1"/>
+    <col min="16132" max="16132" width="19.875" style="4" customWidth="1"/>
+    <col min="16133" max="16133" width="39.625" style="4" customWidth="1"/>
+    <col min="16134" max="16384" width="9" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" ht="46.5" customHeight="1">
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="46.5" customHeight="1">
       <c r="A1" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
-      <c r="D1" s="7"/>
-    </row>
-    <row r="2" spans="1:4" s="1" customFormat="1" ht="18.75">
+      <c r="D1" s="6"/>
+      <c r="E1" s="7"/>
+    </row>
+    <row r="2" spans="1:5" s="1" customFormat="1" ht="18.75">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -839,126 +880,148 @@
         <v>2</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="E2" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="E3" s="3"/>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="E4" s="3"/>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="E5" s="3"/>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="E6" s="3"/>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="E7" s="3"/>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="E8" s="3"/>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
-    </row>
-    <row r="11" spans="1:4">
+      <c r="E10" s="3"/>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="E11" s="3"/>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
-    </row>
-    <row r="13" spans="1:4">
+      <c r="E12" s="3"/>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="E13" s="3"/>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
-    </row>
-    <row r="15" spans="1:4">
+      <c r="E14" s="3"/>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
-    </row>
-    <row r="16" spans="1:4">
+      <c r="E15" s="3"/>
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
-    </row>
-    <row r="17" spans="1:4">
+      <c r="E16" s="3"/>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="E17" s="3"/>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
-    </row>
-    <row r="19" spans="1:4">
+      <c r="E18" s="3"/>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
-    </row>
-    <row r="20" spans="1:4">
+      <c r="E19" s="3"/>
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
-    </row>
-    <row r="21" spans="1:4">
+      <c r="E20" s="3"/>
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A1:E1"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>